<commit_message>
Added description to interactions
</commit_message>
<xml_diff>
--- a/WhyNotExperience-RMA-Workbook.xlsx
+++ b/WhyNotExperience-RMA-Workbook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29602"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petro.kushchak/Library/CloudStorage/Dropbox/_lnu/ooapp/books/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="331" documentId="13_ncr:1_{B1F4C206-CC7E-DD4A-B61E-1CF4A0B74479}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{31E8E622-C457-4C91-A573-44481A60FE86}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{99E8197B-867A-4C96-9D65-CE87AEF79D63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="3640" windowWidth="31000" windowHeight="15340" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1800" yWindow="3640" windowWidth="31000" windowHeight="15340" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Interactions" sheetId="13" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="101">
   <si>
     <t>ID</t>
   </si>
@@ -56,6 +56,30 @@
     <t>Client calls API with GET/PUT/POST HTTP requests</t>
   </si>
   <si>
+    <t>Load Balancer -&gt; API</t>
+  </si>
+  <si>
+    <t>Routes incoming traffic to available API instances and performs regular health checks to ensure upstream availability.</t>
+  </si>
+  <si>
+    <t>API -&gt; Notification Queue</t>
+  </si>
+  <si>
+    <t>Publishes asynchronous messages (booking events, reminders) to the message broker for background processing.</t>
+  </si>
+  <si>
+    <t>API -&gt; DB (PostgreSQL)</t>
+  </si>
+  <si>
+    <t>Executes transactional queries (CRUD) to persist or retrieve core business data (users, events, bookings).</t>
+  </si>
+  <si>
+    <t>API -&gt; Cache DB (Redis)</t>
+  </si>
+  <si>
+    <t>Stores and retrieves frequently accessed data to reduce database load and improve response latency.</t>
+  </si>
+  <si>
     <t>Component / Dependency Interactions</t>
   </si>
   <si>
@@ -155,9 +179,6 @@
     <t>Between 5 min and 45 min</t>
   </si>
   <si>
-    <t>Load Balancer -&gt; API</t>
-  </si>
-  <si>
     <t>Crash::BadGateway (502)</t>
   </si>
   <si>
@@ -191,9 +212,6 @@
     <t>All API instances failed health checks.</t>
   </si>
   <si>
-    <t>API -&gt; Notification Queue</t>
-  </si>
-  <si>
     <t>Omission::BrokerUnreachable</t>
   </si>
   <si>
@@ -224,9 +242,6 @@
     <t>More than 15 min</t>
   </si>
   <si>
-    <t>API -&gt; DB (PostgreSQL)</t>
-  </si>
-  <si>
     <t>Capacity::ConnectionPoolExhausted</t>
   </si>
   <si>
@@ -252,9 +267,6 @@
   </si>
   <si>
     <t>Service fails to start</t>
-  </si>
-  <si>
-    <t>API -&gt; Cache DB (Redis)</t>
   </si>
   <si>
     <t>Capacity::OOM (Out Of Memory)</t>
@@ -1225,9 +1237,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="20% – колірна тема 1" xfId="1" builtinId="30"/>
-    <cellStyle name="Звичайний" xfId="0" builtinId="0"/>
-    <cellStyle name="Фінансовий" xfId="2" builtinId="3"/>
+    <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="27">
     <dxf>
@@ -1994,8 +2006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -2031,29 +2043,45 @@
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="32"/>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="32"/>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="32"/>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="32"/>
+      <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2">
@@ -2114,8 +2142,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N125"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -2140,43 +2168,43 @@
         <v>0</v>
       </c>
       <c r="B1" s="64" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C1" s="64" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D1" s="65" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E1" s="65" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F1" s="66" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="G1" s="66" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="H1" s="66" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="I1" s="66" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="J1" s="67" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="K1" s="68" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="L1" s="74" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="M1" s="29" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="N1" s="29" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="35" customFormat="1" ht="24">
@@ -2184,35 +2212,35 @@
         <v>1</v>
       </c>
       <c r="B2" s="70" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C2" s="70" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="D2" s="71" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="E2" s="70" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="F2" s="72" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="G2" s="72" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="H2" s="72" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="I2" s="72" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="J2" s="72">
         <f>IFERROR(PRODUCT(VLOOKUP(InputTable[[#This Row],[Effects]],WeightTable[[#All],[Effect]:[Weight - Effect]],2,FALSE),VLOOKUP(InputTable[[#This Row],[Portion Affected]],WeightTable[[#All],[% Affected]:[Weight - % Affected]],2,FALSE),SUM(VLOOKUP(InputTable[[#This Row],[Detection]],WeightTable[[#All],[Time to Detect]:[Weight - Detection]],2,FALSE),VLOOKUP(InputTable[[#This Row],[Resolution]],WeightTable[[#All],[Time to Resolve]:[Weight - Resolve]],2,FALSE))),"")</f>
         <v>42</v>
       </c>
       <c r="K2" s="72" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="L2" s="75"/>
       <c r="M2" s="34">
@@ -2229,35 +2257,35 @@
         <v>1</v>
       </c>
       <c r="B3" s="70" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C3" s="70" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="D3" s="71" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="E3" s="70" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="F3" s="72" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="G3" s="72" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="H3" s="72" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" s="72" t="s">
         <v>32</v>
       </c>
-      <c r="I3" s="72" t="s">
-        <v>24</v>
-      </c>
       <c r="J3" s="73">
         <f>IFERROR(PRODUCT(VLOOKUP(InputTable[[#This Row],[Effects]],WeightTable[[#All],[Effect]:[Weight - Effect]],2,FALSE),VLOOKUP(InputTable[[#This Row],[Portion Affected]],WeightTable[[#All],[% Affected]:[Weight - % Affected]],2,FALSE),SUM(VLOOKUP(InputTable[[#This Row],[Detection]],WeightTable[[#All],[Time to Detect]:[Weight - Detection]],2,FALSE),VLOOKUP(InputTable[[#This Row],[Resolution]],WeightTable[[#All],[Time to Resolve]:[Weight - Resolve]],2,FALSE))),"")</f>
         <v>1.5</v>
       </c>
       <c r="K3" s="72" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="L3" s="75"/>
       <c r="M3" s="36">
@@ -2274,35 +2302,35 @@
         <v>1</v>
       </c>
       <c r="B4" s="70" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C4" s="70" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="71" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="70" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="72" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="72" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="72" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="72" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4" s="72">
+        <f>IFERROR(PRODUCT(VLOOKUP(InputTable[[#This Row],[Effects]],WeightTable[[#All],[Effect]:[Weight - Effect]],2,FALSE),VLOOKUP(InputTable[[#This Row],[Portion Affected]],WeightTable[[#All],[% Affected]:[Weight - % Affected]],2,FALSE),SUM(VLOOKUP(InputTable[[#This Row],[Detection]],WeightTable[[#All],[Time to Detect]:[Weight - Detection]],2,FALSE),VLOOKUP(InputTable[[#This Row],[Resolution]],WeightTable[[#All],[Time to Resolve]:[Weight - Resolve]],2,FALSE))),"")</f>
+        <v>31.5</v>
+      </c>
+      <c r="K4" s="72" t="s">
         <v>34</v>
-      </c>
-      <c r="D4" s="71" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" s="70" t="s">
-        <v>36</v>
-      </c>
-      <c r="F4" s="72" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="72" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="72" t="s">
-        <v>24</v>
-      </c>
-      <c r="I4" s="72" t="s">
-        <v>37</v>
-      </c>
-      <c r="J4" s="72">
-        <f>IFERROR(PRODUCT(VLOOKUP(InputTable[[#This Row],[Effects]],WeightTable[[#All],[Effect]:[Weight - Effect]],2,FALSE),VLOOKUP(InputTable[[#This Row],[Portion Affected]],WeightTable[[#All],[% Affected]:[Weight - % Affected]],2,FALSE),SUM(VLOOKUP(InputTable[[#This Row],[Detection]],WeightTable[[#All],[Time to Detect]:[Weight - Detection]],2,FALSE),VLOOKUP(InputTable[[#This Row],[Resolution]],WeightTable[[#All],[Time to Resolve]:[Weight - Resolve]],2,FALSE))),"")</f>
-        <v>31.5</v>
-      </c>
-      <c r="K4" s="72" t="s">
-        <v>26</v>
       </c>
       <c r="L4" s="75"/>
       <c r="M4" s="34">
@@ -2319,35 +2347,35 @@
         <v>2</v>
       </c>
       <c r="B5" s="70" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="C5" s="70" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="D5" s="71" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="E5" s="70" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="F5" s="72" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="G5" s="72" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="H5" s="72" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="I5" s="72" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="J5" s="73">
         <f>IFERROR(PRODUCT(VLOOKUP(InputTable[[#This Row],[Effects]],WeightTable[[#All],[Effect]:[Weight - Effect]],2,FALSE),VLOOKUP(InputTable[[#This Row],[Portion Affected]],WeightTable[[#All],[% Affected]:[Weight - % Affected]],2,FALSE),SUM(VLOOKUP(InputTable[[#This Row],[Detection]],WeightTable[[#All],[Time to Detect]:[Weight - Detection]],2,FALSE),VLOOKUP(InputTable[[#This Row],[Resolution]],WeightTable[[#All],[Time to Resolve]:[Weight - Resolve]],2,FALSE))),"")</f>
         <v>9</v>
       </c>
       <c r="K5" s="72" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="L5" s="75"/>
       <c r="M5" s="34">
@@ -2364,35 +2392,35 @@
         <v>2</v>
       </c>
       <c r="B6" s="70" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="70" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="71" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="70" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" s="72" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="70" t="s">
-        <v>45</v>
-      </c>
-      <c r="D6" s="71" t="s">
-        <v>46</v>
-      </c>
-      <c r="E6" s="70" t="s">
-        <v>47</v>
-      </c>
-      <c r="F6" s="72" t="s">
-        <v>30</v>
-      </c>
       <c r="G6" s="72" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="H6" s="72" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="I6" s="72" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="J6" s="72">
         <f>IFERROR(PRODUCT(VLOOKUP(InputTable[[#This Row],[Effects]],WeightTable[[#All],[Effect]:[Weight - Effect]],2,FALSE),VLOOKUP(InputTable[[#This Row],[Portion Affected]],WeightTable[[#All],[% Affected]:[Weight - % Affected]],2,FALSE),SUM(VLOOKUP(InputTable[[#This Row],[Detection]],WeightTable[[#All],[Time to Detect]:[Weight - Detection]],2,FALSE),VLOOKUP(InputTable[[#This Row],[Resolution]],WeightTable[[#All],[Time to Resolve]:[Weight - Resolve]],2,FALSE))),"")</f>
         <v>5</v>
       </c>
       <c r="K6" s="72" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="L6" s="75"/>
       <c r="M6" s="34">
@@ -2409,35 +2437,35 @@
         <v>2</v>
       </c>
       <c r="B7" s="70" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="C7" s="70" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="D7" s="71" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="E7" s="70" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="F7" s="72" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="G7" s="72" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="H7" s="72" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="I7" s="72" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="J7" s="73">
         <f>IFERROR(PRODUCT(VLOOKUP(InputTable[[#This Row],[Effects]],WeightTable[[#All],[Effect]:[Weight - Effect]],2,FALSE),VLOOKUP(InputTable[[#This Row],[Portion Affected]],WeightTable[[#All],[% Affected]:[Weight - % Affected]],2,FALSE),SUM(VLOOKUP(InputTable[[#This Row],[Detection]],WeightTable[[#All],[Time to Detect]:[Weight - Detection]],2,FALSE),VLOOKUP(InputTable[[#This Row],[Resolution]],WeightTable[[#All],[Time to Resolve]:[Weight - Resolve]],2,FALSE))),"")</f>
         <v>42</v>
       </c>
       <c r="K7" s="72" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="L7" s="75"/>
       <c r="M7" s="34">
@@ -2454,35 +2482,35 @@
         <v>3</v>
       </c>
       <c r="B8" s="70" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="C8" s="70" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="D8" s="71" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="E8" s="70" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="F8" s="72" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="G8" s="72" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="H8" s="72" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="I8" s="72" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="J8" s="72">
         <f>IFERROR(PRODUCT(VLOOKUP(InputTable[[#This Row],[Effects]],WeightTable[[#All],[Effect]:[Weight - Effect]],2,FALSE),VLOOKUP(InputTable[[#This Row],[Portion Affected]],WeightTable[[#All],[% Affected]:[Weight - % Affected]],2,FALSE),SUM(VLOOKUP(InputTable[[#This Row],[Detection]],WeightTable[[#All],[Time to Detect]:[Weight - Detection]],2,FALSE),VLOOKUP(InputTable[[#This Row],[Resolution]],WeightTable[[#All],[Time to Resolve]:[Weight - Resolve]],2,FALSE))),"")</f>
         <v>13.5</v>
       </c>
       <c r="K8" s="72" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="L8" s="75"/>
       <c r="M8" s="34">
@@ -2499,35 +2527,35 @@
         <v>3</v>
       </c>
       <c r="B9" s="70" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="C9" s="70" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="D9" s="71" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E9" s="70" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="F9" s="72" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="G9" s="72" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="H9" s="72" t="s">
+        <v>40</v>
+      </c>
+      <c r="I9" s="72" t="s">
         <v>32</v>
       </c>
-      <c r="I9" s="72" t="s">
-        <v>24</v>
-      </c>
       <c r="J9" s="73">
         <f>IFERROR(PRODUCT(VLOOKUP(InputTable[[#This Row],[Effects]],WeightTable[[#All],[Effect]:[Weight - Effect]],2,FALSE),VLOOKUP(InputTable[[#This Row],[Portion Affected]],WeightTable[[#All],[% Affected]:[Weight - % Affected]],2,FALSE),SUM(VLOOKUP(InputTable[[#This Row],[Detection]],WeightTable[[#All],[Time to Detect]:[Weight - Detection]],2,FALSE),VLOOKUP(InputTable[[#This Row],[Resolution]],WeightTable[[#All],[Time to Resolve]:[Weight - Resolve]],2,FALSE))),"")</f>
         <v>4.5</v>
       </c>
       <c r="K9" s="72" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="L9" s="75"/>
       <c r="M9" s="34">
@@ -2544,35 +2572,35 @@
         <v>3</v>
       </c>
       <c r="B10" s="70" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="C10" s="70" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="D10" s="71" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="E10" s="70" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="F10" s="72" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="G10" s="72" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="H10" s="72" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="I10" s="72" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="J10" s="72">
         <f>IFERROR(PRODUCT(VLOOKUP(InputTable[[#This Row],[Effects]],WeightTable[[#All],[Effect]:[Weight - Effect]],2,FALSE),VLOOKUP(InputTable[[#This Row],[Portion Affected]],WeightTable[[#All],[% Affected]:[Weight - % Affected]],2,FALSE),SUM(VLOOKUP(InputTable[[#This Row],[Detection]],WeightTable[[#All],[Time to Detect]:[Weight - Detection]],2,FALSE),VLOOKUP(InputTable[[#This Row],[Resolution]],WeightTable[[#All],[Time to Resolve]:[Weight - Resolve]],2,FALSE))),"")</f>
         <v>2.5</v>
       </c>
       <c r="K10" s="72" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="L10" s="75"/>
       <c r="M10" s="34">
@@ -2589,35 +2617,35 @@
         <v>4</v>
       </c>
       <c r="B11" s="70" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="C11" s="70" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="D11" s="71" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="E11" s="70" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="F11" s="72" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="G11" s="72" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="H11" s="72" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="I11" s="72" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="J11" s="73">
         <f>IFERROR(PRODUCT(VLOOKUP(InputTable[[#This Row],[Effects]],WeightTable[[#All],[Effect]:[Weight - Effect]],2,FALSE),VLOOKUP(InputTable[[#This Row],[Portion Affected]],WeightTable[[#All],[% Affected]:[Weight - % Affected]],2,FALSE),SUM(VLOOKUP(InputTable[[#This Row],[Detection]],WeightTable[[#All],[Time to Detect]:[Weight - Detection]],2,FALSE),VLOOKUP(InputTable[[#This Row],[Resolution]],WeightTable[[#All],[Time to Resolve]:[Weight - Resolve]],2,FALSE))),"")</f>
         <v>28</v>
       </c>
       <c r="K11" s="72" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="L11" s="75"/>
       <c r="M11" s="34">
@@ -2634,35 +2662,35 @@
         <v>4</v>
       </c>
       <c r="B12" s="70" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="C12" s="70" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="D12" s="71" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="E12" s="70" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="F12" s="72" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="G12" s="72" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="H12" s="72" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="I12" s="72" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="J12" s="72">
         <f>IFERROR(PRODUCT(VLOOKUP(InputTable[[#This Row],[Effects]],WeightTable[[#All],[Effect]:[Weight - Effect]],2,FALSE),VLOOKUP(InputTable[[#This Row],[Portion Affected]],WeightTable[[#All],[% Affected]:[Weight - % Affected]],2,FALSE),SUM(VLOOKUP(InputTable[[#This Row],[Detection]],WeightTable[[#All],[Time to Detect]:[Weight - Detection]],2,FALSE),VLOOKUP(InputTable[[#This Row],[Resolution]],WeightTable[[#All],[Time to Resolve]:[Weight - Resolve]],2,FALSE))),"")</f>
         <v>6</v>
       </c>
       <c r="K12" s="72" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="L12" s="75"/>
       <c r="M12" s="34">
@@ -2679,35 +2707,35 @@
         <v>4</v>
       </c>
       <c r="B13" s="70" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="C13" s="70" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D13" s="71" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="E13" s="70" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="F13" s="72" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="G13" s="72" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="H13" s="72" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="I13" s="72" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="J13" s="73">
         <f>IFERROR(PRODUCT(VLOOKUP(InputTable[[#This Row],[Effects]],WeightTable[[#All],[Effect]:[Weight - Effect]],2,FALSE),VLOOKUP(InputTable[[#This Row],[Portion Affected]],WeightTable[[#All],[% Affected]:[Weight - % Affected]],2,FALSE),SUM(VLOOKUP(InputTable[[#This Row],[Detection]],WeightTable[[#All],[Time to Detect]:[Weight - Detection]],2,FALSE),VLOOKUP(InputTable[[#This Row],[Resolution]],WeightTable[[#All],[Time to Resolve]:[Weight - Resolve]],2,FALSE))),"")</f>
         <v>21</v>
       </c>
       <c r="K13" s="72" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="L13" s="75"/>
       <c r="M13" s="34">
@@ -2724,35 +2752,35 @@
         <v>5</v>
       </c>
       <c r="B14" s="70" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="C14" s="70" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D14" s="71" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="E14" s="70" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F14" s="72" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="G14" s="72" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="H14" s="72" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="I14" s="72" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="J14" s="72">
         <f>IFERROR(PRODUCT(VLOOKUP(InputTable[[#This Row],[Effects]],WeightTable[[#All],[Effect]:[Weight - Effect]],2,FALSE),VLOOKUP(InputTable[[#This Row],[Portion Affected]],WeightTable[[#All],[% Affected]:[Weight - % Affected]],2,FALSE),SUM(VLOOKUP(InputTable[[#This Row],[Detection]],WeightTable[[#All],[Time to Detect]:[Weight - Detection]],2,FALSE),VLOOKUP(InputTable[[#This Row],[Resolution]],WeightTable[[#All],[Time to Resolve]:[Weight - Resolve]],2,FALSE))),"")</f>
         <v>12</v>
       </c>
       <c r="K14" s="72" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="L14" s="75"/>
       <c r="M14" s="34">
@@ -2769,35 +2797,35 @@
         <v>5</v>
       </c>
       <c r="B15" s="70" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="C15" s="70" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D15" s="71" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="E15" s="70" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="F15" s="72" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="G15" s="72" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="H15" s="72" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="I15" s="72" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="J15" s="73">
         <f>IFERROR(PRODUCT(VLOOKUP(InputTable[[#This Row],[Effects]],WeightTable[[#All],[Effect]:[Weight - Effect]],2,FALSE),VLOOKUP(InputTable[[#This Row],[Portion Affected]],WeightTable[[#All],[% Affected]:[Weight - % Affected]],2,FALSE),SUM(VLOOKUP(InputTable[[#This Row],[Detection]],WeightTable[[#All],[Time to Detect]:[Weight - Detection]],2,FALSE),VLOOKUP(InputTable[[#This Row],[Resolution]],WeightTable[[#All],[Time to Resolve]:[Weight - Resolve]],2,FALSE))),"")</f>
         <v>2</v>
       </c>
       <c r="K15" s="72" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="L15" s="75"/>
       <c r="M15" s="34">
@@ -2814,35 +2842,35 @@
         <v>5</v>
       </c>
       <c r="B16" s="70" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="C16" s="70" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D16" s="71" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E16" s="70" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="F16" s="72" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="G16" s="72" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="H16" s="72" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="I16" s="72" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="J16" s="72">
         <f>IFERROR(PRODUCT(VLOOKUP(InputTable[[#This Row],[Effects]],WeightTable[[#All],[Effect]:[Weight - Effect]],2,FALSE),VLOOKUP(InputTable[[#This Row],[Portion Affected]],WeightTable[[#All],[% Affected]:[Weight - % Affected]],2,FALSE),SUM(VLOOKUP(InputTable[[#This Row],[Detection]],WeightTable[[#All],[Time to Detect]:[Weight - Detection]],2,FALSE),VLOOKUP(InputTable[[#This Row],[Resolution]],WeightTable[[#All],[Time to Resolve]:[Weight - Resolve]],2,FALSE))),"")</f>
         <v>18</v>
       </c>
       <c r="K16" s="72" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="L16" s="75"/>
       <c r="M16" s="34">
@@ -5276,50 +5304,50 @@
   <sheetData>
     <row r="1" spans="2:13">
       <c r="B1" s="26" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="2:13" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="B2" s="3" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="I2" s="14" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="J2" s="16" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="K2" s="17" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="L2" s="18" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="M2" s="19" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="2:13" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="B3" s="5" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C3" s="6">
         <v>0</v>
@@ -5337,115 +5365,115 @@
     </row>
     <row r="4" spans="2:13" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="B4" s="5" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="C4" s="6">
         <v>1</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="E4" s="6">
         <v>1</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="G4" s="6">
         <v>0.5</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="I4" s="6">
         <v>0.5</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="K4" s="6">
         <v>1</v>
       </c>
       <c r="L4" s="20" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="M4" s="21"/>
     </row>
     <row r="5" spans="2:13" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="B5" s="5" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="C5" s="6">
         <v>3</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="E5" s="6">
         <v>2</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="G5" s="6">
         <v>1</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="I5" s="6">
         <v>1</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="K5" s="6">
         <v>2</v>
       </c>
       <c r="L5" s="20" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="M5" s="21"/>
     </row>
     <row r="6" spans="2:13" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="B6" s="7" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="C6" s="8">
         <v>7</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="E6" s="8">
         <v>3</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="G6" s="8">
         <v>1.5</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="I6" s="8">
         <v>1.5</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="K6" s="8">
         <v>3</v>
       </c>
       <c r="L6" s="22" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="M6" s="23"/>
     </row>
     <row r="8" spans="2:13">
       <c r="B8" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -5458,6 +5486,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="c1928375-0f1f-4f90-a126-ff5ee6140227" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00de483d-de58-4028-9f3a-56464c66a56c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Документ" ma:contentTypeID="0x01010058C87C40172A324BABA0D20EA6D226DF" ma:contentTypeVersion="11" ma:contentTypeDescription="Створення нового документа." ma:contentTypeScope="" ma:versionID="aaeb852ab7e279cd65c00d4ae04e8482">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00de483d-de58-4028-9f3a-56464c66a56c" xmlns:ns3="c1928375-0f1f-4f90-a126-ff5ee6140227" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8739bdd35a5363ac3dabb80f3da36ba5" ns2:_="" ns3:_="">
     <xsd:import namespace="00de483d-de58-4028-9f3a-56464c66a56c"/>
@@ -5652,28 +5700,8 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="c1928375-0f1f-4f90-a126-ff5ee6140227" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00de483d-de58-4028-9f3a-56464c66a56c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED513E42-7148-4D9A-864D-17DB4A4F1EEE}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C8C7842-1BD8-44B3-8E36-554202982C10}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5681,5 +5709,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C8C7842-1BD8-44B3-8E36-554202982C10}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED513E42-7148-4D9A-864D-17DB4A4F1EEE}"/>
 </file>
</xml_diff>